<commit_message>
KPIs voor probleem 2
</commit_message>
<xml_diff>
--- a/Group8_results.xlsx
+++ b/Group8_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\GitHub\airlineplanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E574E8D5-C390-4FAA-8453-52C074BA85DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D14FDB-47E9-411F-95A5-870F95F00967}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="21576" windowHeight="10224" activeTab="1" xr2:uid="{0837EA09-EFE8-486C-BBF5-C9418E4164D4}"/>
   </bookViews>
@@ -4162,7 +4162,7 @@
         <v>3</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -4174,7 +4174,7 @@
         <v>16</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -4588,7 +4588,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -4884,7 +4884,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -5772,7 +5772,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -5790,7 +5790,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -5914,7 +5914,7 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -5938,7 +5938,7 @@
         <v>3</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -6077,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -6148,7 +6148,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -6358,13 +6358,13 @@
     </row>
     <row r="33" spans="1:24">
       <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
         <v>2</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -6468,7 +6468,7 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -6681,7 +6681,7 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>

</xml_diff>

<commit_message>
problem 1 en 2
</commit_message>
<xml_diff>
--- a/Group8_results.xlsx
+++ b/Group8_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\GitHub\airlineplanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A361D4C4-DF4E-41AE-8B73-20E34B5DF4F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C1E247-EA5A-42C8-80DE-9D3425330217}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="21576" windowHeight="10224" activeTab="1" xr2:uid="{0837EA09-EFE8-486C-BBF5-C9418E4164D4}"/>
   </bookViews>
@@ -4162,7 +4162,7 @@
         <v>3</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -4174,7 +4174,7 @@
         <v>16</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -4588,7 +4588,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -4884,7 +4884,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -5772,7 +5772,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -5790,7 +5790,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -5914,7 +5914,7 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -5938,7 +5938,7 @@
         <v>3</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -6077,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -6148,7 +6148,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -6358,13 +6358,13 @@
     </row>
     <row r="33" spans="1:24">
       <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
         <v>2</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -6468,7 +6468,7 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -6681,7 +6681,7 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>

</xml_diff>

<commit_message>
probleem 3 volledig gefixed
</commit_message>
<xml_diff>
--- a/Group8_results.xlsx
+++ b/Group8_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\GitHub\airlineplanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F706D873-BC96-4C5E-A808-54C52B3B017E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676AFDC8-8555-475A-88B1-6E71E2894897}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="21576" windowHeight="10224" activeTab="1" xr2:uid="{0837EA09-EFE8-486C-BBF5-C9418E4164D4}"/>
   </bookViews>
@@ -4162,7 +4162,7 @@
         <v>3</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -4174,7 +4174,7 @@
         <v>16</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -4588,7 +4588,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -4884,7 +4884,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -5772,7 +5772,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -5790,7 +5790,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -5914,7 +5914,7 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -5938,7 +5938,7 @@
         <v>3</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -6077,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -6148,7 +6148,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -6358,13 +6358,13 @@
     </row>
     <row r="33" spans="1:24">
       <c r="A33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -6468,7 +6468,7 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -6681,7 +6681,7 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37">
         <v>0</v>

</xml_diff>